<commit_message>
Revert "update meeting log"
This reverts commit 2abd082f8a2ace31637dcd32b67efa8990dc5cde.
</commit_message>
<xml_diff>
--- a/meetingLog.xlsx
+++ b/meetingLog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
   <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -259,12 +259,6 @@
   </si>
   <si>
     <t>fixed bugs</t>
-  </si>
-  <si>
-    <t>regression test</t>
-  </si>
-  <si>
-    <t>2/12</t>
   </si>
 </sst>
 </file>
@@ -748,7 +742,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1222,21 +1216,11 @@
       <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7">

</xml_diff>

<commit_message>
Revert "Revert "update meeting log""
This reverts commit 7ace7517378a8acbe22ea75a633eb86636bb6077.
</commit_message>
<xml_diff>
--- a/meetingLog.xlsx
+++ b/meetingLog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
   <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>fixed bugs</t>
+  </si>
+  <si>
+    <t>regression test</t>
+  </si>
+  <si>
+    <t>2/12</t>
   </si>
 </sst>
 </file>
@@ -742,7 +748,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1216,11 +1222,21 @@
       <c r="A23" s="4">
         <v>21</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="2"/>
+      <c r="B23" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7">

</xml_diff>